<commit_message>
# 9 form de descto o ingreso de empleados
</commit_message>
<xml_diff>
--- a/Lista de Pantallas/Lista de Pantallas.xlsx
+++ b/Lista de Pantallas/Lista de Pantallas.xlsx
@@ -48,9 +48,6 @@
     <t>Lista de acumulados básicos</t>
   </si>
   <si>
-    <t>Datos Generales ( 10)</t>
-  </si>
-  <si>
     <t>Acumulados (8)</t>
   </si>
   <si>
@@ -214,6 +211,9 @@
   </si>
   <si>
     <t>cierre anual</t>
+  </si>
+  <si>
+    <t>Datos Generales ( 10) - 1</t>
   </si>
 </sst>
 </file>
@@ -272,10 +272,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -572,8 +572,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -583,15 +583,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
-      <c r="A1" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+      <c r="A1" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
     </row>
     <row r="3" spans="1:7">
       <c r="A3" s="3" t="s">
@@ -647,23 +647,23 @@
       <c r="A10" s="2">
         <v>1</v>
       </c>
-      <c r="B10" t="s">
-        <v>10</v>
+      <c r="B10" s="4" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7">
       <c r="A11" s="2">
         <v>2</v>
       </c>
-      <c r="B11" s="5" t="s">
-        <v>11</v>
+      <c r="B11" s="4" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="12" spans="1:7">
       <c r="A12" s="2">
         <v>3</v>
       </c>
-      <c r="B12" t="s">
+      <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
     </row>
@@ -671,8 +671,8 @@
       <c r="A13" s="2">
         <v>4</v>
       </c>
-      <c r="B13" t="s">
-        <v>12</v>
+      <c r="B13" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -688,7 +688,7 @@
         <v>6</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="16" spans="1:7">
@@ -704,12 +704,12 @@
         <v>8</v>
       </c>
       <c r="B17" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="18" spans="1:2">
       <c r="A18" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:2">
@@ -717,7 +717,7 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="20" spans="1:2">
@@ -725,7 +725,7 @@
         <v>2</v>
       </c>
       <c r="B20" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="21" spans="1:2">
@@ -733,7 +733,7 @@
         <v>3</v>
       </c>
       <c r="B21" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2">
@@ -741,7 +741,7 @@
         <v>4</v>
       </c>
       <c r="B22" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:2">
@@ -749,7 +749,7 @@
         <v>5</v>
       </c>
       <c r="B23" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="24" spans="1:2">
@@ -757,7 +757,7 @@
         <v>6</v>
       </c>
       <c r="B24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:2">
@@ -765,12 +765,12 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="26" spans="1:2">
       <c r="A26" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="27" spans="1:2">
@@ -778,7 +778,7 @@
         <v>1</v>
       </c>
       <c r="B27" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2">
@@ -786,7 +786,7 @@
         <v>2</v>
       </c>
       <c r="B28" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2">
@@ -794,7 +794,7 @@
         <v>3</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:2">
@@ -802,12 +802,12 @@
         <v>4</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="1" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="32" spans="1:2">
@@ -815,7 +815,7 @@
         <v>1</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="33" spans="1:2">
@@ -823,7 +823,7 @@
         <v>2</v>
       </c>
       <c r="B33" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:2">
@@ -831,7 +831,7 @@
         <v>3</v>
       </c>
       <c r="B34" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="35" spans="1:2">
@@ -839,7 +839,7 @@
         <v>4</v>
       </c>
       <c r="B35" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="36" spans="1:2">
@@ -847,12 +847,12 @@
         <v>5</v>
       </c>
       <c r="B36" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="37" spans="1:2">
       <c r="A37" s="3" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="38" spans="1:2">
@@ -860,7 +860,7 @@
         <v>1</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:2">
@@ -868,7 +868,7 @@
         <v>2</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:2">
@@ -876,7 +876,7 @@
         <v>3</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2">
@@ -884,7 +884,7 @@
         <v>4</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:2">
@@ -892,7 +892,7 @@
         <v>5</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:2">
@@ -900,7 +900,7 @@
         <v>6</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -908,7 +908,7 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:2">
@@ -916,12 +916,12 @@
         <v>8</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:2">
       <c r="A46" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="47" spans="1:2">
@@ -929,7 +929,7 @@
         <v>1</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="48" spans="1:2">
@@ -937,7 +937,7 @@
         <v>2</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="49" spans="1:3">
@@ -945,7 +945,7 @@
         <v>3</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="50" spans="1:3">
@@ -953,7 +953,7 @@
         <v>4</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="51" spans="1:3">
@@ -961,7 +961,7 @@
         <v>5</v>
       </c>
       <c r="B51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="52" spans="1:3">
@@ -969,7 +969,7 @@
         <v>6</v>
       </c>
       <c r="B52" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="53" spans="1:3">
@@ -977,12 +977,12 @@
         <v>7</v>
       </c>
       <c r="B53" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="54" spans="1:3">
       <c r="A54" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:3">
@@ -990,10 +990,10 @@
         <v>1</v>
       </c>
       <c r="B55" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C55" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="56" spans="1:3">
@@ -1001,12 +1001,12 @@
         <v>2</v>
       </c>
       <c r="B56" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="57" spans="1:3">
       <c r="A57" s="1" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="58" spans="1:3">
@@ -1014,7 +1014,7 @@
         <v>1</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="59" spans="1:3">
@@ -1022,7 +1022,7 @@
         <v>2</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:3">
@@ -1030,7 +1030,7 @@
         <v>3</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:3">
@@ -1038,7 +1038,7 @@
         <v>4</v>
       </c>
       <c r="B61" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:3">
@@ -1046,7 +1046,7 @@
         <v>5</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:3">
@@ -1054,7 +1054,7 @@
         <v>6</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:3">
@@ -1062,7 +1062,7 @@
         <v>7</v>
       </c>
       <c r="B64" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -1070,7 +1070,7 @@
         <v>8</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -1078,7 +1078,7 @@
         <v>9</v>
       </c>
       <c r="B66" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
#  15 consumiendo servicios para el calculo de planilla
</commit_message>
<xml_diff>
--- a/Lista de Pantallas/Lista de Pantallas.xlsx
+++ b/Lista de Pantallas/Lista de Pantallas.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="70">
   <si>
     <t>Inicio</t>
   </si>
@@ -214,6 +214,18 @@
   </si>
   <si>
     <t>Datos Generales ( 10) - 1</t>
+  </si>
+  <si>
+    <t>tablas  que considero ue faltan</t>
+  </si>
+  <si>
+    <t>acredores</t>
+  </si>
+  <si>
+    <t>secciones</t>
+  </si>
+  <si>
+    <t>departamentos</t>
   </si>
 </sst>
 </file>
@@ -572,8 +584,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:G66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -679,7 +691,7 @@
       <c r="A14" s="2">
         <v>5</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B14" s="4" t="s">
         <v>8</v>
       </c>
     </row>
@@ -732,7 +744,7 @@
       <c r="A21" s="2">
         <v>3</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="4" t="s">
         <v>17</v>
       </c>
     </row>
@@ -740,7 +752,7 @@
       <c r="A22" s="2">
         <v>4</v>
       </c>
-      <c r="B22" t="s">
+      <c r="B22" s="4" t="s">
         <v>18</v>
       </c>
     </row>
@@ -748,7 +760,7 @@
       <c r="A23" s="2">
         <v>5</v>
       </c>
-      <c r="B23" t="s">
+      <c r="B23" s="4" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1092,12 +1104,77 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:B11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="14.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2">
+      <c r="A10">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2">
+      <c r="A11">
+        <v>9</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>

</xml_diff>